<commit_message>
feat: bug fixes and footnotes
</commit_message>
<xml_diff>
--- a/output/Тренировка.xlsx
+++ b/output/Тренировка.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Content\Проекты\AzimuthGrid\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786FA100-7DC5-4366-B404-5AF21FC62006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56750985-429C-4078-B130-EB5170A4BC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,8 +415,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -759,41 +759,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58:F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="3"/>
+    <col min="1" max="1" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
       <c r="D2" t="s">
         <v>6</v>
       </c>
@@ -803,11 +803,11 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3">
@@ -816,12 +816,21 @@
       <c r="C3">
         <v>277</v>
       </c>
+      <c r="D3">
+        <v>91</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>600</v>
+      </c>
       <c r="H3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4">
@@ -834,8 +843,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
@@ -848,8 +857,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6">
@@ -862,8 +871,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
@@ -876,8 +885,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8">
@@ -890,8 +899,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9">
@@ -900,12 +909,15 @@
       <c r="C9">
         <v>69</v>
       </c>
+      <c r="G9">
+        <v>190</v>
+      </c>
       <c r="H9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10">
@@ -914,12 +926,21 @@
       <c r="C10">
         <v>233</v>
       </c>
+      <c r="D10">
+        <v>91</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>600</v>
+      </c>
       <c r="H10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11">
@@ -932,8 +953,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12">
@@ -946,8 +967,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -960,8 +981,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
@@ -974,8 +995,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15">
@@ -988,8 +1009,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16">
@@ -998,12 +1019,15 @@
       <c r="C16">
         <v>161</v>
       </c>
+      <c r="G16">
+        <v>332</v>
+      </c>
       <c r="H16">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B17">
@@ -1012,12 +1036,21 @@
       <c r="C17">
         <v>138</v>
       </c>
+      <c r="D17">
+        <v>91</v>
+      </c>
+      <c r="E17">
+        <v>50</v>
+      </c>
+      <c r="F17">
+        <v>600</v>
+      </c>
       <c r="H17">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B18">
@@ -1030,8 +1063,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B19">
@@ -1044,8 +1077,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B20">
@@ -1058,8 +1091,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B21">
@@ -1072,8 +1105,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B22">
@@ -1082,12 +1115,15 @@
       <c r="C22">
         <v>57</v>
       </c>
+      <c r="G22">
+        <v>190</v>
+      </c>
       <c r="H22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B23">
@@ -1096,12 +1132,21 @@
       <c r="C23">
         <v>191</v>
       </c>
+      <c r="D23">
+        <v>91</v>
+      </c>
+      <c r="E23">
+        <v>50</v>
+      </c>
+      <c r="F23">
+        <v>600</v>
+      </c>
       <c r="H23">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B24">
@@ -1114,8 +1159,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B25">
@@ -1128,8 +1173,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B26">
@@ -1142,8 +1187,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B27">
@@ -1156,8 +1201,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B28">
@@ -1166,12 +1211,15 @@
       <c r="C28">
         <v>41</v>
       </c>
+      <c r="G28">
+        <v>192</v>
+      </c>
       <c r="H28">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B29">
@@ -1180,12 +1228,21 @@
       <c r="C29">
         <v>290</v>
       </c>
+      <c r="D29">
+        <v>91</v>
+      </c>
+      <c r="E29">
+        <v>50</v>
+      </c>
+      <c r="F29">
+        <v>600</v>
+      </c>
       <c r="H29">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B30">
@@ -1198,8 +1255,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B31">
@@ -1212,8 +1269,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B32">
@@ -1226,8 +1283,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B33">
@@ -1240,8 +1297,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B34">
@@ -1254,8 +1311,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B35">
@@ -1264,12 +1321,15 @@
       <c r="C35">
         <v>100</v>
       </c>
+      <c r="G35">
+        <v>190</v>
+      </c>
       <c r="H35">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B36">
@@ -1278,12 +1338,21 @@
       <c r="C36">
         <v>291</v>
       </c>
+      <c r="D36">
+        <v>91</v>
+      </c>
+      <c r="E36">
+        <v>50</v>
+      </c>
+      <c r="F36">
+        <v>600</v>
+      </c>
       <c r="H36">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B37">
@@ -1296,8 +1365,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B38">
@@ -1310,8 +1379,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B39">
@@ -1324,8 +1393,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B40">
@@ -1338,8 +1407,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B41">
@@ -1352,8 +1421,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B42">
@@ -1366,8 +1435,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B43">
@@ -1380,8 +1449,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B44">
@@ -1394,8 +1463,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B45">
@@ -1408,8 +1477,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B46">
@@ -1418,12 +1487,15 @@
       <c r="C46">
         <v>174</v>
       </c>
+      <c r="G46">
+        <v>192</v>
+      </c>
       <c r="H46">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B47">
@@ -1432,12 +1504,21 @@
       <c r="C47">
         <v>271</v>
       </c>
+      <c r="D47">
+        <v>91</v>
+      </c>
+      <c r="E47">
+        <v>50</v>
+      </c>
+      <c r="F47">
+        <v>600</v>
+      </c>
       <c r="H47">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B48">
@@ -1450,8 +1531,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B49">
@@ -1464,8 +1545,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B50">
@@ -1478,8 +1559,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B51">
@@ -1492,8 +1573,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B52">
@@ -1506,8 +1587,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B53">
@@ -1520,8 +1601,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B54">
@@ -1534,8 +1615,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B55">
@@ -1548,8 +1629,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B56">
@@ -1562,8 +1643,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B57">
@@ -1572,12 +1653,15 @@
       <c r="C57">
         <v>99</v>
       </c>
+      <c r="G57">
+        <v>192</v>
+      </c>
       <c r="H57">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B58">
@@ -1586,12 +1670,21 @@
       <c r="C58">
         <v>182</v>
       </c>
+      <c r="D58">
+        <v>91</v>
+      </c>
+      <c r="E58">
+        <v>70</v>
+      </c>
+      <c r="F58">
+        <v>1200</v>
+      </c>
       <c r="H58">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B59">
@@ -1604,8 +1697,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B60">
@@ -1618,8 +1711,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B61">
@@ -1632,8 +1725,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B62">
@@ -1642,12 +1735,15 @@
       <c r="C62">
         <v>122</v>
       </c>
+      <c r="G62">
+        <v>192</v>
+      </c>
       <c r="H62">
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B63">
@@ -1656,12 +1752,21 @@
       <c r="C63">
         <v>180</v>
       </c>
+      <c r="D63">
+        <v>91</v>
+      </c>
+      <c r="E63">
+        <v>50</v>
+      </c>
+      <c r="F63">
+        <v>600</v>
+      </c>
       <c r="H63">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B64">
@@ -1674,8 +1779,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B65">
@@ -1688,8 +1793,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B66">
@@ -1702,8 +1807,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B67">
@@ -1716,8 +1821,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B68">
@@ -1730,8 +1835,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B69">
@@ -1740,12 +1845,15 @@
       <c r="C69">
         <v>118</v>
       </c>
+      <c r="G69">
+        <v>190</v>
+      </c>
       <c r="H69">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B70">
@@ -1754,12 +1862,21 @@
       <c r="C70">
         <v>124</v>
       </c>
+      <c r="D70">
+        <v>91</v>
+      </c>
+      <c r="E70">
+        <v>50</v>
+      </c>
+      <c r="F70">
+        <v>600</v>
+      </c>
       <c r="H70">
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B71">
@@ -1772,8 +1889,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B72">
@@ -1786,8 +1903,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B73">
@@ -1800,8 +1917,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B74">
@@ -1814,8 +1931,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B75">
@@ -1828,8 +1945,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B76">
@@ -1842,8 +1959,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B77">
@@ -1856,8 +1973,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B78">
@@ -1870,8 +1987,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B79">
@@ -1884,8 +2001,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B80">
@@ -1898,8 +2015,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B81">
@@ -1912,8 +2029,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B82">
@@ -1926,8 +2043,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B83">
@@ -1940,8 +2057,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B84">
@@ -1954,8 +2071,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B85">
@@ -1968,8 +2085,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B86">
@@ -1982,8 +2099,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B87">
@@ -1996,8 +2113,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B88">
@@ -2010,8 +2127,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B89">
@@ -2024,8 +2141,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B90">
@@ -2038,8 +2155,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B91">
@@ -2052,8 +2169,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B92">
@@ -2066,8 +2183,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B93">
@@ -2080,8 +2197,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B94">
@@ -2089,6 +2206,9 @@
       </c>
       <c r="C94">
         <v>91</v>
+      </c>
+      <c r="G94">
+        <v>332</v>
       </c>
       <c r="H94">
         <v>91</v>
@@ -2105,7 +2225,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:H94" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H2 A11:H15 A9:F9 H9 A18:H21 A16:F16 H16 A24:H27 A22:F22 H22 A30:H34 A28:F28 H28 A37:H45 A35:F35 H35 A48:H56 A46:F46 H46 A59:H61 A57:F57 H57 A64:H68 A62:F62 H62 A71:H93 A69:F69 H69 A94:F94 H94 A4:H8 A3:C3 G3:H3 A10:C10 G10:H10 A17:C17 G17:H17 A23:C23 G23:H23 A29:C29 G29:H29 A36:C36 G36:H36 A47:C47 G47:H47 A58:C58 G58:H58 A63:C63 G63:H63 A70:C70 G70:H70" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2114,46 +2234,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58:H58"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="2"/>
       <c r="F2" t="s">
         <v>6</v>
       </c>
@@ -2163,10 +2285,10 @@
       <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2182,11 +2304,20 @@
       <c r="E3" t="s">
         <v>32</v>
       </c>
+      <c r="F3">
+        <v>91</v>
+      </c>
+      <c r="G3">
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <v>600</v>
+      </c>
       <c r="J3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2206,7 +2337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2226,7 +2357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2246,7 +2377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2266,7 +2397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2286,7 +2417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2302,11 +2433,14 @@
       <c r="E9" t="s">
         <v>38</v>
       </c>
+      <c r="I9">
+        <v>190</v>
+      </c>
       <c r="J9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2322,11 +2456,20 @@
       <c r="E10" t="s">
         <v>39</v>
       </c>
+      <c r="F10">
+        <v>91</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <v>600</v>
+      </c>
       <c r="J10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2346,7 +2489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2366,7 +2509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2386,7 +2529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2406,7 +2549,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2426,7 +2569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2442,11 +2585,14 @@
       <c r="E16" t="s">
         <v>45</v>
       </c>
+      <c r="I16">
+        <v>332</v>
+      </c>
       <c r="J16">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2462,11 +2608,20 @@
       <c r="E17" t="s">
         <v>46</v>
       </c>
+      <c r="F17">
+        <v>91</v>
+      </c>
+      <c r="G17">
+        <v>50</v>
+      </c>
+      <c r="H17">
+        <v>600</v>
+      </c>
       <c r="J17">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2486,7 +2641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2506,7 +2661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -2526,7 +2681,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -2546,7 +2701,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2562,11 +2717,14 @@
       <c r="E22" t="s">
         <v>51</v>
       </c>
+      <c r="I22">
+        <v>192</v>
+      </c>
       <c r="J22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -2582,11 +2740,20 @@
       <c r="E23" t="s">
         <v>52</v>
       </c>
+      <c r="F23">
+        <v>91</v>
+      </c>
+      <c r="G23">
+        <v>50</v>
+      </c>
+      <c r="H23">
+        <v>600</v>
+      </c>
       <c r="J23">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -2606,7 +2773,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -2626,7 +2793,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -2646,7 +2813,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -2666,7 +2833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2682,11 +2849,14 @@
       <c r="E28" t="s">
         <v>57</v>
       </c>
+      <c r="I28">
+        <v>192</v>
+      </c>
       <c r="J28">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2702,11 +2872,20 @@
       <c r="E29" t="s">
         <v>58</v>
       </c>
+      <c r="F29">
+        <v>91</v>
+      </c>
+      <c r="G29">
+        <v>50</v>
+      </c>
+      <c r="H29">
+        <v>600</v>
+      </c>
       <c r="J29">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -2726,7 +2905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -2746,7 +2925,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2766,7 +2945,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -2786,7 +2965,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -2806,7 +2985,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -2822,11 +3001,14 @@
       <c r="E35" t="s">
         <v>63</v>
       </c>
+      <c r="I35">
+        <v>192</v>
+      </c>
       <c r="J35">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -2842,11 +3024,20 @@
       <c r="E36" t="s">
         <v>64</v>
       </c>
+      <c r="F36">
+        <v>91</v>
+      </c>
+      <c r="G36">
+        <v>50</v>
+      </c>
+      <c r="H36">
+        <v>600</v>
+      </c>
       <c r="J36">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -2866,7 +3057,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -2886,7 +3077,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -2906,7 +3097,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -2926,7 +3117,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -2946,7 +3137,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -2966,7 +3157,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -2986,7 +3177,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -3006,7 +3197,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -3026,7 +3217,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -3042,11 +3233,14 @@
       <c r="E46" t="s">
         <v>74</v>
       </c>
+      <c r="I46">
+        <v>192</v>
+      </c>
       <c r="J46">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -3062,11 +3256,20 @@
       <c r="E47" t="s">
         <v>75</v>
       </c>
+      <c r="F47">
+        <v>91</v>
+      </c>
+      <c r="G47">
+        <v>50</v>
+      </c>
+      <c r="H47">
+        <v>600</v>
+      </c>
       <c r="J47">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -3086,7 +3289,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -3106,7 +3309,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -3126,7 +3329,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -3146,7 +3349,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -3166,7 +3369,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>22</v>
       </c>
@@ -3186,7 +3389,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -3206,7 +3409,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -3226,7 +3429,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>22</v>
       </c>
@@ -3246,7 +3449,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -3262,11 +3465,14 @@
       <c r="E57" t="s">
         <v>82</v>
       </c>
+      <c r="I57">
+        <v>192</v>
+      </c>
       <c r="J57">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -3282,11 +3488,20 @@
       <c r="E58" t="s">
         <v>83</v>
       </c>
+      <c r="F58">
+        <v>91</v>
+      </c>
+      <c r="G58">
+        <v>70</v>
+      </c>
+      <c r="H58">
+        <v>1200</v>
+      </c>
       <c r="J58">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -3306,7 +3521,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>24</v>
       </c>
@@ -3326,7 +3541,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>24</v>
       </c>
@@ -3346,7 +3561,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -3362,11 +3577,14 @@
       <c r="E62" t="s">
         <v>87</v>
       </c>
+      <c r="I62">
+        <v>192</v>
+      </c>
       <c r="J62">
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>25</v>
       </c>
@@ -3382,11 +3600,20 @@
       <c r="E63" t="s">
         <v>88</v>
       </c>
+      <c r="F63">
+        <v>91</v>
+      </c>
+      <c r="G63">
+        <v>50</v>
+      </c>
+      <c r="H63">
+        <v>600</v>
+      </c>
       <c r="J63">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -3406,7 +3633,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -3426,7 +3653,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>26</v>
       </c>
@@ -3446,7 +3673,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -3466,7 +3693,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -3486,7 +3713,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -3502,11 +3729,14 @@
       <c r="E69" t="s">
         <v>94</v>
       </c>
+      <c r="I69">
+        <v>192</v>
+      </c>
       <c r="J69">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>27</v>
       </c>
@@ -3522,11 +3752,20 @@
       <c r="E70" t="s">
         <v>95</v>
       </c>
+      <c r="F70">
+        <v>91</v>
+      </c>
+      <c r="G70">
+        <v>50</v>
+      </c>
+      <c r="H70">
+        <v>600</v>
+      </c>
       <c r="J70">
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -3546,7 +3785,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -3566,7 +3805,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -3586,7 +3825,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -3606,7 +3845,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>28</v>
       </c>
@@ -3626,7 +3865,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -3646,7 +3885,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>28</v>
       </c>
@@ -3666,7 +3905,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>28</v>
       </c>
@@ -3686,7 +3925,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>28</v>
       </c>
@@ -3706,7 +3945,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>28</v>
       </c>
@@ -3726,7 +3965,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>28</v>
       </c>
@@ -3746,7 +3985,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>28</v>
       </c>
@@ -3766,7 +4005,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>28</v>
       </c>
@@ -3786,7 +4025,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>28</v>
       </c>
@@ -3806,7 +4045,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>28</v>
       </c>
@@ -3826,7 +4065,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>28</v>
       </c>
@@ -3846,7 +4085,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>28</v>
       </c>
@@ -3866,7 +4105,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>28</v>
       </c>
@@ -3886,7 +4125,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>28</v>
       </c>
@@ -3906,7 +4145,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>28</v>
       </c>
@@ -3926,7 +4165,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>28</v>
       </c>
@@ -3946,7 +4185,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>28</v>
       </c>
@@ -3966,7 +4205,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>28</v>
       </c>
@@ -3986,7 +4225,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>28</v>
       </c>
@@ -4001,6 +4240,9 @@
       </c>
       <c r="E94" t="s">
         <v>118</v>
+      </c>
+      <c r="I94">
+        <v>332</v>
       </c>
       <c r="J94">
         <v>91</v>
@@ -4018,7 +4260,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:J94" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H2 J1:J94 A4:H9 A3:E3 A11:H16 A10:E10 A18:H22 A17:E17 A24:H28 A23:E23 A30:H35 A29:E29 A37:H46 A36:E36 A48:H57 A47:E47 A59:H62 A58:E58 A64:H69 A63:E63 A71:H94 A70:E70" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>